<commit_message>
Add exported anomaly tables and CSV results
</commit_message>
<xml_diff>
--- a/projet capstone/results/tables/anomaly_A1_by_ticker.xlsx
+++ b/projet capstone/results/tables/anomaly_A1_by_ticker.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -495,7 +495,7 @@
         <v>0.03270173200076178</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4673913043478261</v>
+        <v>0.4951690821256038</v>
       </c>
       <c r="F2" t="n">
         <v>828</v>
@@ -522,7 +522,7 @@
         <v>0.03241249196062459</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4951690821256038</v>
+        <v>0.4927536231884058</v>
       </c>
       <c r="F3" t="n">
         <v>828</v>
@@ -549,7 +549,7 @@
         <v>0.03499560181538106</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4927536231884058</v>
+        <v>0.46256038647343</v>
       </c>
       <c r="F4" t="n">
         <v>828</v>
@@ -576,7 +576,7 @@
         <v>0.03517566880533739</v>
       </c>
       <c r="E5" t="n">
-        <v>0.46256038647343</v>
+        <v>0.4589371980676328</v>
       </c>
       <c r="F5" t="n">
         <v>828</v>
@@ -603,7 +603,7 @@
         <v>0.03794661579536783</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4583835946924005</v>
+        <v>0.4668275030156815</v>
       </c>
       <c r="F6" t="n">
         <v>828</v>
@@ -630,7 +630,7 @@
         <v>0.02443170720958026</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4565217391304348</v>
+        <v>0.5048309178743962</v>
       </c>
       <c r="F7" t="n">
         <v>828</v>
@@ -657,7 +657,7 @@
         <v>0.02623838007095019</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5048309178743962</v>
+        <v>0.4794685990338164</v>
       </c>
       <c r="F8" t="n">
         <v>828</v>
@@ -684,7 +684,7 @@
         <v>0.02734255729674243</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4794685990338164</v>
+        <v>0.4879227053140097</v>
       </c>
       <c r="F9" t="n">
         <v>828</v>
@@ -711,7 +711,7 @@
         <v>0.02759802647671843</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4879227053140097</v>
+        <v>0.5157004830917874</v>
       </c>
       <c r="F10" t="n">
         <v>828</v>
@@ -738,7 +738,7 @@
         <v>0.02342196370914277</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5150784077201448</v>
+        <v>0.4559710494571773</v>
       </c>
       <c r="F11" t="n">
         <v>828</v>
@@ -765,7 +765,7 @@
         <v>0.02454697365129225</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4408212560386474</v>
+        <v>0.4927536231884058</v>
       </c>
       <c r="F12" t="n">
         <v>828</v>
@@ -792,7 +792,7 @@
         <v>0.02418178563526392</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4927536231884058</v>
+        <v>0.4794685990338164</v>
       </c>
       <c r="F13" t="n">
         <v>828</v>
@@ -819,7 +819,7 @@
         <v>0.0242546494295428</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4794685990338164</v>
+        <v>0.5048309178743962</v>
       </c>
       <c r="F14" t="n">
         <v>828</v>
@@ -846,7 +846,7 @@
         <v>0.03830552950544799</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5048309178743962</v>
+        <v>0.4673913043478261</v>
       </c>
       <c r="F15" t="n">
         <v>828</v>
@@ -873,7 +873,7 @@
         <v>0.0293173785739047</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4668275030156815</v>
+        <v>0.4402895054282268</v>
       </c>
       <c r="F16" t="n">
         <v>828</v>
@@ -900,7 +900,7 @@
         <v>0.03668169620774981</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4045893719806763</v>
+        <v>0.4842995169082125</v>
       </c>
       <c r="F17" t="n">
         <v>828</v>
@@ -927,7 +927,7 @@
         <v>0.03098452675494484</v>
       </c>
       <c r="E18" t="n">
-        <v>0.4842995169082125</v>
+        <v>0.4528985507246377</v>
       </c>
       <c r="F18" t="n">
         <v>828</v>
@@ -954,7 +954,7 @@
         <v>0.02954544901357071</v>
       </c>
       <c r="E19" t="n">
-        <v>0.4528985507246377</v>
+        <v>0.4842995169082125</v>
       </c>
       <c r="F19" t="n">
         <v>828</v>
@@ -981,7 +981,7 @@
         <v>0.02953893413310067</v>
       </c>
       <c r="E20" t="n">
-        <v>0.4842995169082125</v>
+        <v>0.4734299516908212</v>
       </c>
       <c r="F20" t="n">
         <v>828</v>
@@ -1008,7 +1008,7 @@
         <v>0.02858064313510895</v>
       </c>
       <c r="E21" t="n">
-        <v>0.4728588661037395</v>
+        <v>0.4041013268998794</v>
       </c>
       <c r="F21" t="n">
         <v>828</v>
@@ -1035,7 +1035,7 @@
         <v>0.02711090613084628</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4504830917874396</v>
+        <v>0.5289855072463768</v>
       </c>
       <c r="F22" t="n">
         <v>828</v>
@@ -1062,7 +1062,7 @@
         <v>0.02768837498956683</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5289855072463768</v>
+        <v>0.4879227053140097</v>
       </c>
       <c r="F23" t="n">
         <v>828</v>
@@ -1089,7 +1089,7 @@
         <v>0.03621350903443172</v>
       </c>
       <c r="E24" t="n">
-        <v>0.4879227053140097</v>
+        <v>0.5132850241545893</v>
       </c>
       <c r="F24" t="n">
         <v>828</v>
@@ -1116,7 +1116,7 @@
         <v>0.03095320141284885</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5132850241545893</v>
+        <v>0.4698067632850241</v>
       </c>
       <c r="F25" t="n">
         <v>828</v>
@@ -1143,7 +1143,7 @@
         <v>0.03027992700389392</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4692400482509047</v>
+        <v>0.4499396863691194</v>
       </c>
       <c r="F26" t="n">
         <v>828</v>
@@ -1170,7 +1170,7 @@
         <v>0.03942301949994417</v>
       </c>
       <c r="E27" t="n">
-        <v>0.463768115942029</v>
+        <v>0.5120772946859904</v>
       </c>
       <c r="F27" t="n">
         <v>828</v>
@@ -1197,7 +1197,7 @@
         <v>0.03432250526912907</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5120772946859904</v>
+        <v>0.4842995169082125</v>
       </c>
       <c r="F28" t="n">
         <v>828</v>
@@ -1224,7 +1224,7 @@
         <v>0.03085849990565951</v>
       </c>
       <c r="E29" t="n">
-        <v>0.4842995169082125</v>
+        <v>0.498792270531401</v>
       </c>
       <c r="F29" t="n">
         <v>828</v>
@@ -1251,7 +1251,7 @@
         <v>0.0322187003837844</v>
       </c>
       <c r="E30" t="n">
-        <v>0.498792270531401</v>
+        <v>0.4685990338164251</v>
       </c>
       <c r="F30" t="n">
         <v>828</v>
@@ -1278,7 +1278,7 @@
         <v>0.0323181239124922</v>
       </c>
       <c r="E31" t="n">
-        <v>0.4680337756332931</v>
+        <v>0.4632086851628468</v>
       </c>
       <c r="F31" t="n">
         <v>828</v>
@@ -1305,7 +1305,7 @@
         <v>0.03078026533951659</v>
       </c>
       <c r="E32" t="n">
-        <v>0.4347826086956522</v>
+        <v>0.5084541062801933</v>
       </c>
       <c r="F32" t="n">
         <v>828</v>
@@ -1332,7 +1332,7 @@
         <v>0.02879379272883474</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5084541062801933</v>
+        <v>0.4903381642512077</v>
       </c>
       <c r="F33" t="n">
         <v>828</v>
@@ -1359,7 +1359,7 @@
         <v>0.03126589253443803</v>
       </c>
       <c r="E34" t="n">
-        <v>0.4903381642512077</v>
+        <v>0.4818840579710145</v>
       </c>
       <c r="F34" t="n">
         <v>828</v>
@@ -1386,7 +1386,7 @@
         <v>0.02874308295316029</v>
       </c>
       <c r="E35" t="n">
-        <v>0.4818840579710145</v>
+        <v>0.4782608695652174</v>
       </c>
       <c r="F35" t="n">
         <v>828</v>
@@ -1413,7 +1413,7 @@
         <v>0.02896661469608075</v>
       </c>
       <c r="E36" t="n">
-        <v>0.4776839565741858</v>
+        <v>0.4342581423401689</v>
       </c>
       <c r="F36" t="n">
         <v>828</v>
@@ -1440,7 +1440,7 @@
         <v>0.02325937147945116</v>
       </c>
       <c r="E37" t="n">
-        <v>0.4698067632850241</v>
+        <v>0.5084541062801933</v>
       </c>
       <c r="F37" t="n">
         <v>828</v>
@@ -1467,7 +1467,7 @@
         <v>0.02343950950677185</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5084541062801933</v>
+        <v>0.4963768115942029</v>
       </c>
       <c r="F38" t="n">
         <v>828</v>
@@ -1494,7 +1494,7 @@
         <v>0.02435383936762955</v>
       </c>
       <c r="E39" t="n">
-        <v>0.4963768115942029</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="F39" t="n">
         <v>828</v>
@@ -1521,7 +1521,7 @@
         <v>0.02562657166371877</v>
       </c>
       <c r="E40" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5048309178743962</v>
       </c>
       <c r="F40" t="n">
         <v>828</v>
@@ -1548,7 +1548,7 @@
         <v>0.03591945026371354</v>
       </c>
       <c r="E41" t="n">
-        <v>0.5042219541616405</v>
+        <v>0.4692400482509047</v>
       </c>
       <c r="F41" t="n">
         <v>828</v>
@@ -1575,7 +1575,7 @@
         <v>0.02918480662934756</v>
       </c>
       <c r="E42" t="n">
-        <v>0.4154589371980676</v>
+        <v>0.4915458937198068</v>
       </c>
       <c r="F42" t="n">
         <v>828</v>
@@ -1602,7 +1602,7 @@
         <v>0.02615789862191673</v>
       </c>
       <c r="E43" t="n">
-        <v>0.4915458937198068</v>
+        <v>0.46256038647343</v>
       </c>
       <c r="F43" t="n">
         <v>828</v>
@@ -1629,7 +1629,7 @@
         <v>0.03045626070063105</v>
       </c>
       <c r="E44" t="n">
-        <v>0.46256038647343</v>
+        <v>0.4601449275362319</v>
       </c>
       <c r="F44" t="n">
         <v>828</v>
@@ -1656,7 +1656,7 @@
         <v>0.0263822816474588</v>
       </c>
       <c r="E45" t="n">
-        <v>0.4601449275362319</v>
+        <v>0.4528985507246377</v>
       </c>
       <c r="F45" t="n">
         <v>828</v>
@@ -1683,7 +1683,7 @@
         <v>0.02668703402931631</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4523522316043426</v>
+        <v>0.4149577804583836</v>
       </c>
       <c r="F46" t="n">
         <v>828</v>
@@ -1710,7 +1710,7 @@
         <v>0.02532769385598432</v>
       </c>
       <c r="E47" t="n">
-        <v>0.4601449275362319</v>
+        <v>0.5217391304347826</v>
       </c>
       <c r="F47" t="n">
         <v>828</v>
@@ -1737,7 +1737,7 @@
         <v>0.0248350806521264</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5217391304347826</v>
+        <v>0.5024154589371981</v>
       </c>
       <c r="F48" t="n">
         <v>828</v>
@@ -1764,7 +1764,7 @@
         <v>0.0268801870022784</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5024154589371981</v>
+        <v>0.4685990338164251</v>
       </c>
       <c r="F49" t="n">
         <v>828</v>
@@ -1791,7 +1791,7 @@
         <v>0.0351213883933607</v>
       </c>
       <c r="E50" t="n">
-        <v>0.4685990338164251</v>
+        <v>0.5072463768115942</v>
       </c>
       <c r="F50" t="n">
         <v>828</v>
@@ -1818,7 +1818,7 @@
         <v>0.03370380913800147</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5066344993968637</v>
+        <v>0.4595898673100121</v>
       </c>
       <c r="F51" t="n">
         <v>828</v>
@@ -1845,7 +1845,7 @@
         <v>0.02863998669861477</v>
       </c>
       <c r="E52" t="n">
-        <v>0.4408212560386474</v>
+        <v>0.4867149758454106</v>
       </c>
       <c r="F52" t="n">
         <v>828</v>
@@ -1872,7 +1872,7 @@
         <v>0.02506152986329764</v>
       </c>
       <c r="E53" t="n">
-        <v>0.4867149758454106</v>
+        <v>0.4468599033816425</v>
       </c>
       <c r="F53" t="n">
         <v>828</v>
@@ -1899,7 +1899,7 @@
         <v>0.02523873240988815</v>
       </c>
       <c r="E54" t="n">
-        <v>0.4468599033816425</v>
+        <v>0.4601449275362319</v>
       </c>
       <c r="F54" t="n">
         <v>828</v>
@@ -1926,7 +1926,7 @@
         <v>0.02730392258528682</v>
       </c>
       <c r="E55" t="n">
-        <v>0.4601449275362319</v>
+        <v>0.46256038647343</v>
       </c>
       <c r="F55" t="n">
         <v>828</v>
@@ -1953,7 +1953,7 @@
         <v>0.02785106545575029</v>
       </c>
       <c r="E56" t="n">
-        <v>0.4620024125452352</v>
+        <v>0.4402895054282268</v>
       </c>
       <c r="F56" t="n">
         <v>828</v>
@@ -1980,7 +1980,7 @@
         <v>0.02336492229830405</v>
       </c>
       <c r="E57" t="n">
-        <v>0.4263285024154589</v>
+        <v>0.5483091787439613</v>
       </c>
       <c r="F57" t="n">
         <v>828</v>
@@ -2007,7 +2007,7 @@
         <v>0.0211744863198634</v>
       </c>
       <c r="E58" t="n">
-        <v>0.5483091787439613</v>
+        <v>0.4673913043478261</v>
       </c>
       <c r="F58" t="n">
         <v>828</v>
@@ -2034,7 +2034,7 @@
         <v>0.02251767659909406</v>
       </c>
       <c r="E59" t="n">
-        <v>0.4673913043478261</v>
+        <v>0.4685990338164251</v>
       </c>
       <c r="F59" t="n">
         <v>828</v>
@@ -2061,7 +2061,7 @@
         <v>0.02608408105018058</v>
       </c>
       <c r="E60" t="n">
-        <v>0.4685990338164251</v>
+        <v>0.4963768115942029</v>
       </c>
       <c r="F60" t="n">
         <v>828</v>
@@ -2088,7 +2088,7 @@
         <v>0.03400817788541984</v>
       </c>
       <c r="E61" t="n">
-        <v>0.4957780458383595</v>
+        <v>0.4258142340168878</v>
       </c>
       <c r="F61" t="n">
         <v>828</v>
@@ -2115,7 +2115,7 @@
         <v>0.02875553747987073</v>
       </c>
       <c r="E62" t="n">
-        <v>0.4456521739130435</v>
+        <v>0.4879227053140097</v>
       </c>
       <c r="F62" t="n">
         <v>828</v>
@@ -2142,7 +2142,7 @@
         <v>0.03726444291772619</v>
       </c>
       <c r="E63" t="n">
-        <v>0.4879227053140097</v>
+        <v>0.4830917874396135</v>
       </c>
       <c r="F63" t="n">
         <v>828</v>
@@ -2169,7 +2169,7 @@
         <v>0.03529043973230857</v>
       </c>
       <c r="E64" t="n">
-        <v>0.4830917874396135</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="F64" t="n">
         <v>828</v>
@@ -2196,7 +2196,7 @@
         <v>0.03237034241147013</v>
       </c>
       <c r="E65" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4420289855072464</v>
       </c>
       <c r="F65" t="n">
         <v>828</v>
@@ -2223,7 +2223,7 @@
         <v>0.03308906264938725</v>
       </c>
       <c r="E66" t="n">
-        <v>0.4414957780458383</v>
+        <v>0.4451145958986731</v>
       </c>
       <c r="F66" t="n">
         <v>828</v>
@@ -2250,7 +2250,7 @@
         <v>0.02177497983088111</v>
       </c>
       <c r="E67" t="n">
-        <v>0.463768115942029</v>
+        <v>0.498792270531401</v>
       </c>
       <c r="F67" t="n">
         <v>828</v>
@@ -2277,7 +2277,7 @@
         <v>0.0220199621166969</v>
       </c>
       <c r="E68" t="n">
-        <v>0.498792270531401</v>
+        <v>0.5120772946859904</v>
       </c>
       <c r="F68" t="n">
         <v>828</v>
@@ -2304,7 +2304,7 @@
         <v>0.02604511865683792</v>
       </c>
       <c r="E69" t="n">
-        <v>0.5120772946859904</v>
+        <v>0.5181159420289855</v>
       </c>
       <c r="F69" t="n">
         <v>828</v>
@@ -2331,7 +2331,7 @@
         <v>0.02963221896207887</v>
       </c>
       <c r="E70" t="n">
-        <v>0.5181159420289855</v>
+        <v>0.5289855072463768</v>
       </c>
       <c r="F70" t="n">
         <v>828</v>
@@ -2358,7 +2358,7 @@
         <v>0.02774194339277637</v>
       </c>
       <c r="E71" t="n">
-        <v>0.5283474065138721</v>
+        <v>0.4632086851628468</v>
       </c>
       <c r="F71" t="n">
         <v>828</v>
@@ -2385,7 +2385,7 @@
         <v>0.02824524709375115</v>
       </c>
       <c r="E72" t="n">
-        <v>0.4492753623188406</v>
+        <v>0.4818840579710145</v>
       </c>
       <c r="F72" t="n">
         <v>828</v>
@@ -2412,7 +2412,7 @@
         <v>0.03219394102199544</v>
       </c>
       <c r="E73" t="n">
-        <v>0.4818840579710145</v>
+        <v>0.4734299516908212</v>
       </c>
       <c r="F73" t="n">
         <v>828</v>
@@ -2439,7 +2439,7 @@
         <v>0.0331869418419904</v>
       </c>
       <c r="E74" t="n">
-        <v>0.4734299516908212</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="F74" t="n">
         <v>828</v>
@@ -2466,7 +2466,7 @@
         <v>0.03135300428366965</v>
       </c>
       <c r="E75" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.4673913043478261</v>
       </c>
       <c r="F75" t="n">
         <v>828</v>
@@ -2493,7 +2493,7 @@
         <v>0.02788439783128052</v>
       </c>
       <c r="E76" t="n">
-        <v>0.4668275030156815</v>
+        <v>0.4487334137515078</v>
       </c>
       <c r="F76" t="n">
         <v>828</v>
@@ -2514,16 +2514,16 @@
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.00163510396400472</v>
+        <v>0.001647039029435411</v>
       </c>
       <c r="D77" t="n">
-        <v>0.02499365743641477</v>
+        <v>0.02508442771410914</v>
       </c>
       <c r="E77" t="n">
-        <v>0.4661835748792271</v>
+        <v>0.4768856447688564</v>
       </c>
       <c r="F77" t="n">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2541,16 +2541,16 @@
         <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>0.0005913616826931194</v>
+        <v>0.0005956781913259159</v>
       </c>
       <c r="D78" t="n">
-        <v>0.02641939906540035</v>
+        <v>0.02651571339068073</v>
       </c>
       <c r="E78" t="n">
-        <v>0.4758454106280193</v>
+        <v>0.4744525547445255</v>
       </c>
       <c r="F78" t="n">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2568,16 +2568,16 @@
         <v>2</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0007897906292512543</v>
+        <v>0.000795555524355278</v>
       </c>
       <c r="D79" t="n">
-        <v>0.03148587973034446</v>
+        <v>0.03160064957136633</v>
       </c>
       <c r="E79" t="n">
-        <v>0.4746376811594203</v>
+        <v>0.4963503649635037</v>
       </c>
       <c r="F79" t="n">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2595,16 +2595,16 @@
         <v>3</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0007488376422112585</v>
+        <v>0.0007543036104025815</v>
       </c>
       <c r="D80" t="n">
-        <v>0.02754006848122476</v>
+        <v>0.02764044423903863</v>
       </c>
       <c r="E80" t="n">
-        <v>0.4963768115942029</v>
+        <v>0.4933171324422843</v>
       </c>
       <c r="F80" t="n">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2622,16 +2622,16 @@
         <v>4</v>
       </c>
       <c r="C81" t="n">
-        <v>0.0009884661345211895</v>
+        <v>0.0009944713965778188</v>
       </c>
       <c r="D81" t="n">
-        <v>0.02198442991619127</v>
+        <v>0.02205105559018989</v>
       </c>
       <c r="E81" t="n">
-        <v>0.4933655006031363</v>
+        <v>0.4665856622114216</v>
       </c>
       <c r="F81" t="n">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -2655,7 +2655,7 @@
         <v>0.02972724376737183</v>
       </c>
       <c r="E82" t="n">
-        <v>0.4251207729468599</v>
+        <v>0.4806763285024155</v>
       </c>
       <c r="F82" t="n">
         <v>828</v>
@@ -2682,7 +2682,7 @@
         <v>0.02570638671418367</v>
       </c>
       <c r="E83" t="n">
-        <v>0.4806763285024155</v>
+        <v>0.4661835748792271</v>
       </c>
       <c r="F83" t="n">
         <v>828</v>
@@ -2709,7 +2709,7 @@
         <v>0.02764135560861283</v>
       </c>
       <c r="E84" t="n">
-        <v>0.4661835748792271</v>
+        <v>0.4794685990338164</v>
       </c>
       <c r="F84" t="n">
         <v>828</v>
@@ -2736,7 +2736,7 @@
         <v>0.02486123832985858</v>
       </c>
       <c r="E85" t="n">
-        <v>0.4794685990338164</v>
+        <v>0.4661835748792271</v>
       </c>
       <c r="F85" t="n">
         <v>828</v>
@@ -2763,7 +2763,7 @@
         <v>0.02388962567896621</v>
       </c>
       <c r="E86" t="n">
-        <v>0.46562123039807</v>
+        <v>0.4246079613992763</v>
       </c>
       <c r="F86" t="n">
         <v>828</v>
@@ -2790,7 +2790,7 @@
         <v>0.02442728967493618</v>
       </c>
       <c r="E87" t="n">
-        <v>0.4541062801932367</v>
+        <v>0.4830917874396135</v>
       </c>
       <c r="F87" t="n">
         <v>828</v>
@@ -2817,7 +2817,7 @@
         <v>0.02276952871319072</v>
       </c>
       <c r="E88" t="n">
-        <v>0.4830917874396135</v>
+        <v>0.4867149758454106</v>
       </c>
       <c r="F88" t="n">
         <v>828</v>
@@ -2871,7 +2871,7 @@
         <v>0.02826117828879142</v>
       </c>
       <c r="E90" t="n">
-        <v>0.4867149758454106</v>
+        <v>0.4746376811594203</v>
       </c>
       <c r="F90" t="n">
         <v>828</v>
@@ -2898,7 +2898,7 @@
         <v>0.02905723735279385</v>
       </c>
       <c r="E91" t="n">
-        <v>0.474065138721351</v>
+        <v>0.4535585042219542</v>
       </c>
       <c r="F91" t="n">
         <v>828</v>
@@ -2925,7 +2925,7 @@
         <v>0.02897733051355603</v>
       </c>
       <c r="E92" t="n">
-        <v>0.4384057971014493</v>
+        <v>0.5229468599033816</v>
       </c>
       <c r="F92" t="n">
         <v>828</v>
@@ -2952,7 +2952,7 @@
         <v>0.02858253877139159</v>
       </c>
       <c r="E93" t="n">
-        <v>0.5229468599033816</v>
+        <v>0.4698067632850241</v>
       </c>
       <c r="F93" t="n">
         <v>828</v>
@@ -2979,7 +2979,7 @@
         <v>0.02745832209988046</v>
       </c>
       <c r="E94" t="n">
-        <v>0.4698067632850241</v>
+        <v>0.4867149758454106</v>
       </c>
       <c r="F94" t="n">
         <v>828</v>
@@ -3006,7 +3006,7 @@
         <v>0.02916370933003725</v>
       </c>
       <c r="E95" t="n">
-        <v>0.4867149758454106</v>
+        <v>0.4758454106280193</v>
       </c>
       <c r="F95" t="n">
         <v>828</v>
@@ -3033,7 +3033,7 @@
         <v>0.02425996204836758</v>
       </c>
       <c r="E96" t="n">
-        <v>0.4752714113389626</v>
+        <v>0.4378769601930036</v>
       </c>
       <c r="F96" t="n">
         <v>828</v>
@@ -3060,7 +3060,7 @@
         <v>0.02814455898817664</v>
       </c>
       <c r="E97" t="n">
-        <v>0.4251207729468599</v>
+        <v>0.5314009661835749</v>
       </c>
       <c r="F97" t="n">
         <v>828</v>
@@ -3087,7 +3087,7 @@
         <v>0.02894849183619666</v>
       </c>
       <c r="E98" t="n">
-        <v>0.5314009661835749</v>
+        <v>0.4927536231884058</v>
       </c>
       <c r="F98" t="n">
         <v>828</v>
@@ -3114,7 +3114,7 @@
         <v>0.03092446930654819</v>
       </c>
       <c r="E99" t="n">
-        <v>0.4927536231884058</v>
+        <v>0.5084541062801933</v>
       </c>
       <c r="F99" t="n">
         <v>828</v>
@@ -3141,7 +3141,7 @@
         <v>0.03167794085657266</v>
       </c>
       <c r="E100" t="n">
-        <v>0.5084541062801933</v>
+        <v>0.4565217391304348</v>
       </c>
       <c r="F100" t="n">
         <v>828</v>
@@ -3168,7 +3168,7 @@
         <v>0.02916973614843422</v>
       </c>
       <c r="E101" t="n">
-        <v>0.4559710494571773</v>
+        <v>0.4246079613992763</v>
       </c>
       <c r="F101" t="n">
         <v>828</v>
@@ -3195,7 +3195,7 @@
         <v>0.02515413986368158</v>
       </c>
       <c r="E102" t="n">
-        <v>0.4468599033816425</v>
+        <v>0.5132850241545893</v>
       </c>
       <c r="F102" t="n">
         <v>828</v>
@@ -3222,7 +3222,7 @@
         <v>0.02591056311605961</v>
       </c>
       <c r="E103" t="n">
-        <v>0.5132850241545893</v>
+        <v>0.5205314009661836</v>
       </c>
       <c r="F103" t="n">
         <v>828</v>
@@ -3249,7 +3249,7 @@
         <v>0.02607221542187976</v>
       </c>
       <c r="E104" t="n">
-        <v>0.5205314009661836</v>
+        <v>0.5036231884057971</v>
       </c>
       <c r="F104" t="n">
         <v>828</v>
@@ -3276,7 +3276,7 @@
         <v>0.02787815850557068</v>
       </c>
       <c r="E105" t="n">
-        <v>0.5036231884057971</v>
+        <v>0.5120772946859904</v>
       </c>
       <c r="F105" t="n">
         <v>828</v>
@@ -3303,7 +3303,7 @@
         <v>0.02630492961399514</v>
       </c>
       <c r="E106" t="n">
-        <v>0.51145958986731</v>
+        <v>0.4463208685162847</v>
       </c>
       <c r="F106" t="n">
         <v>828</v>
@@ -3330,7 +3330,7 @@
         <v>0.02533221650868854</v>
       </c>
       <c r="E107" t="n">
-        <v>0.4577294685990338</v>
+        <v>0.5072463768115942</v>
       </c>
       <c r="F107" t="n">
         <v>828</v>
@@ -3357,7 +3357,7 @@
         <v>0.0318262183778566</v>
       </c>
       <c r="E108" t="n">
-        <v>0.5072463768115942</v>
+        <v>0.5157004830917874</v>
       </c>
       <c r="F108" t="n">
         <v>828</v>
@@ -3384,7 +3384,7 @@
         <v>0.0326174323996172</v>
       </c>
       <c r="E109" t="n">
-        <v>0.5157004830917874</v>
+        <v>0.4661835748792271</v>
       </c>
       <c r="F109" t="n">
         <v>828</v>
@@ -3411,7 +3411,7 @@
         <v>0.03573858156937999</v>
       </c>
       <c r="E110" t="n">
-        <v>0.4661835748792271</v>
+        <v>0.4565217391304348</v>
       </c>
       <c r="F110" t="n">
         <v>828</v>
@@ -3438,7 +3438,7 @@
         <v>0.02539109842231253</v>
       </c>
       <c r="E111" t="n">
-        <v>0.4559710494571773</v>
+        <v>0.4571773220747889</v>
       </c>
       <c r="F111" t="n">
         <v>828</v>
@@ -3465,7 +3465,7 @@
         <v>0.02750821418375641</v>
       </c>
       <c r="E112" t="n">
-        <v>0.4782608695652174</v>
+        <v>0.5157004830917874</v>
       </c>
       <c r="F112" t="n">
         <v>828</v>
@@ -3492,7 +3492,7 @@
         <v>0.02646336825072433</v>
       </c>
       <c r="E113" t="n">
-        <v>0.5157004830917874</v>
+        <v>0.5084541062801933</v>
       </c>
       <c r="F113" t="n">
         <v>828</v>
@@ -3519,7 +3519,7 @@
         <v>0.02750021309823095</v>
       </c>
       <c r="E114" t="n">
-        <v>0.5084541062801933</v>
+        <v>0.5132850241545893</v>
       </c>
       <c r="F114" t="n">
         <v>828</v>
@@ -3546,7 +3546,7 @@
         <v>0.03021512635874792</v>
       </c>
       <c r="E115" t="n">
-        <v>0.5132850241545893</v>
+        <v>0.4613526570048309</v>
       </c>
       <c r="F115" t="n">
         <v>828</v>
@@ -3573,7 +3573,7 @@
         <v>0.02981152042510506</v>
       </c>
       <c r="E116" t="n">
-        <v>0.4607961399276236</v>
+        <v>0.4776839565741858</v>
       </c>
       <c r="F116" t="n">
         <v>828</v>
@@ -3594,16 +3594,16 @@
         <v>0</v>
       </c>
       <c r="C117" t="n">
-        <v>0.0002052037951617267</v>
+        <v>0.0002131853731416684</v>
       </c>
       <c r="D117" t="n">
-        <v>0.02463015812066981</v>
+        <v>0.02510515076842376</v>
       </c>
       <c r="E117" t="n">
-        <v>0.4420289855072464</v>
+        <v>0.4981179422835634</v>
       </c>
       <c r="F117" t="n">
-        <v>828</v>
+        <v>797</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -3621,16 +3621,16 @@
         <v>1</v>
       </c>
       <c r="C118" t="n">
-        <v>0.002008899486444905</v>
+        <v>0.002087037358565096</v>
       </c>
       <c r="D118" t="n">
-        <v>0.02488536901795581</v>
+        <v>0.02536209888871419</v>
       </c>
       <c r="E118" t="n">
-        <v>0.4939613526570048</v>
+        <v>0.4968632371392723</v>
       </c>
       <c r="F118" t="n">
-        <v>828</v>
+        <v>797</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -3648,16 +3648,16 @@
         <v>2</v>
       </c>
       <c r="C119" t="n">
-        <v>0.001529987900656907</v>
+        <v>0.001589498095036285</v>
       </c>
       <c r="D119" t="n">
-        <v>0.02701575893151985</v>
+        <v>0.02753507535729439</v>
       </c>
       <c r="E119" t="n">
-        <v>0.498792270531401</v>
+        <v>0.4717691342534505</v>
       </c>
       <c r="F119" t="n">
-        <v>828</v>
+        <v>797</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -3675,16 +3675,16 @@
         <v>3</v>
       </c>
       <c r="C120" t="n">
-        <v>0.0006480617340561731</v>
+        <v>0.0006732686521938661</v>
       </c>
       <c r="D120" t="n">
-        <v>0.0282522879714424</v>
+        <v>0.02879687728502739</v>
       </c>
       <c r="E120" t="n">
-        <v>0.4698067632850241</v>
+        <v>0.4780426599749059</v>
       </c>
       <c r="F120" t="n">
-        <v>828</v>
+        <v>797</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -3702,16 +3702,16 @@
         <v>4</v>
       </c>
       <c r="C121" t="n">
-        <v>0.0004614616624440137</v>
+        <v>0.0004794106104186241</v>
       </c>
       <c r="D121" t="n">
-        <v>0.02406908478164926</v>
+        <v>0.02453311469395227</v>
       </c>
       <c r="E121" t="n">
-        <v>0.4776839565741858</v>
+        <v>0.4461152882205514</v>
       </c>
       <c r="F121" t="n">
-        <v>828</v>
+        <v>797</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -3735,7 +3735,7 @@
         <v>0.03171126674760194</v>
       </c>
       <c r="E122" t="n">
-        <v>0.4178743961352657</v>
+        <v>0.4758454106280193</v>
       </c>
       <c r="F122" t="n">
         <v>828</v>
@@ -3762,7 +3762,7 @@
         <v>0.02346664197576094</v>
       </c>
       <c r="E123" t="n">
-        <v>0.4758454106280193</v>
+        <v>0.4396135265700483</v>
       </c>
       <c r="F123" t="n">
         <v>828</v>
@@ -3789,7 +3789,7 @@
         <v>0.02429791057906323</v>
       </c>
       <c r="E124" t="n">
-        <v>0.4396135265700483</v>
+        <v>0.463768115942029</v>
       </c>
       <c r="F124" t="n">
         <v>828</v>
@@ -3816,7 +3816,7 @@
         <v>0.02350360361052389</v>
       </c>
       <c r="E125" t="n">
-        <v>0.463768115942029</v>
+        <v>0.4746376811594203</v>
       </c>
       <c r="F125" t="n">
         <v>828</v>
@@ -3843,7 +3843,7 @@
         <v>0.02612064127646924</v>
       </c>
       <c r="E126" t="n">
-        <v>0.474065138721351</v>
+        <v>0.4173703256936068</v>
       </c>
       <c r="F126" t="n">
         <v>828</v>
@@ -3870,7 +3870,7 @@
         <v>0.03014755144165747</v>
       </c>
       <c r="E127" t="n">
-        <v>0.4698067632850241</v>
+        <v>0.5120772946859904</v>
       </c>
       <c r="F127" t="n">
         <v>828</v>
@@ -3897,7 +3897,7 @@
         <v>0.02612075417877808</v>
       </c>
       <c r="E128" t="n">
-        <v>0.5120772946859904</v>
+        <v>0.5024154589371981</v>
       </c>
       <c r="F128" t="n">
         <v>828</v>
@@ -3924,7 +3924,7 @@
         <v>0.02943770024773412</v>
       </c>
       <c r="E129" t="n">
-        <v>0.5024154589371981</v>
+        <v>0.4504830917874396</v>
       </c>
       <c r="F129" t="n">
         <v>828</v>
@@ -3951,7 +3951,7 @@
         <v>0.02942909075114711</v>
       </c>
       <c r="E130" t="n">
-        <v>0.4504830917874396</v>
+        <v>0.4842995169082125</v>
       </c>
       <c r="F130" t="n">
         <v>828</v>
@@ -3978,7 +3978,7 @@
         <v>0.02591912523074536</v>
       </c>
       <c r="E131" t="n">
-        <v>0.4837153196622437</v>
+        <v>0.4692400482509047</v>
       </c>
       <c r="F131" t="n">
         <v>828</v>
@@ -4005,7 +4005,7 @@
         <v>0.02397312246660337</v>
       </c>
       <c r="E132" t="n">
-        <v>0.4130434782608696</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="F132" t="n">
         <v>828</v>
@@ -4032,7 +4032,7 @@
         <v>0.0250950410409952</v>
       </c>
       <c r="E133" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4891304347826087</v>
       </c>
       <c r="F133" t="n">
         <v>828</v>
@@ -4059,7 +4059,7 @@
         <v>0.02929592134068195</v>
       </c>
       <c r="E134" t="n">
-        <v>0.4891304347826087</v>
+        <v>0.4830917874396135</v>
       </c>
       <c r="F134" t="n">
         <v>828</v>
@@ -4086,7 +4086,7 @@
         <v>0.02816851195907011</v>
       </c>
       <c r="E135" t="n">
-        <v>0.4830917874396135</v>
+        <v>0.4842995169082125</v>
       </c>
       <c r="F135" t="n">
         <v>828</v>
@@ -4113,7 +4113,7 @@
         <v>0.02603081454875854</v>
       </c>
       <c r="E136" t="n">
-        <v>0.4837153196622437</v>
+        <v>0.4125452352231604</v>
       </c>
       <c r="F136" t="n">
         <v>828</v>
@@ -4140,7 +4140,7 @@
         <v>0.03237260772285423</v>
       </c>
       <c r="E137" t="n">
-        <v>0.4106280193236715</v>
+        <v>0.4867149758454106</v>
       </c>
       <c r="F137" t="n">
         <v>828</v>
@@ -4167,7 +4167,7 @@
         <v>0.02495207850131354</v>
       </c>
       <c r="E138" t="n">
-        <v>0.4867149758454106</v>
+        <v>0.4782608695652174</v>
       </c>
       <c r="F138" t="n">
         <v>828</v>
@@ -4194,7 +4194,7 @@
         <v>0.02490016409142808</v>
       </c>
       <c r="E139" t="n">
-        <v>0.4782608695652174</v>
+        <v>0.4710144927536232</v>
       </c>
       <c r="F139" t="n">
         <v>828</v>
@@ -4221,7 +4221,7 @@
         <v>0.03693700925845818</v>
       </c>
       <c r="E140" t="n">
-        <v>0.4710144927536232</v>
+        <v>0.501207729468599</v>
       </c>
       <c r="F140" t="n">
         <v>828</v>
@@ -4248,7 +4248,7 @@
         <v>0.02822627486241401</v>
       </c>
       <c r="E141" t="n">
-        <v>0.5006031363088058</v>
+        <v>0.4101326899879373</v>
       </c>
       <c r="F141" t="n">
         <v>828</v>
@@ -4275,7 +4275,7 @@
         <v>0.03040909842794681</v>
       </c>
       <c r="E142" t="n">
-        <v>0.4432367149758454</v>
+        <v>0.5217391304347826</v>
       </c>
       <c r="F142" t="n">
         <v>828</v>
@@ -4302,7 +4302,7 @@
         <v>0.0298234249743622</v>
       </c>
       <c r="E143" t="n">
-        <v>0.5217391304347826</v>
+        <v>0.4867149758454106</v>
       </c>
       <c r="F143" t="n">
         <v>828</v>
@@ -4356,7 +4356,7 @@
         <v>0.03010078395873867</v>
       </c>
       <c r="E145" t="n">
-        <v>0.4867149758454106</v>
+        <v>0.4698067632850241</v>
       </c>
       <c r="F145" t="n">
         <v>828</v>
@@ -4383,7 +4383,7 @@
         <v>0.02754728968453724</v>
       </c>
       <c r="E146" t="n">
-        <v>0.4692400482509047</v>
+        <v>0.4427020506634499</v>
       </c>
       <c r="F146" t="n">
         <v>828</v>
@@ -4410,7 +4410,7 @@
         <v>0.02198742025399425</v>
       </c>
       <c r="E147" t="n">
-        <v>0.4746376811594203</v>
+        <v>0.4903381642512077</v>
       </c>
       <c r="F147" t="n">
         <v>828</v>
@@ -4437,7 +4437,7 @@
         <v>0.02586613156317069</v>
       </c>
       <c r="E148" t="n">
-        <v>0.4903381642512077</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="F148" t="n">
         <v>828</v>
@@ -4464,7 +4464,7 @@
         <v>0.02625894740886672</v>
       </c>
       <c r="E149" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.5108695652173914</v>
       </c>
       <c r="F149" t="n">
         <v>828</v>
@@ -4491,7 +4491,7 @@
         <v>0.02768284855662644</v>
       </c>
       <c r="E150" t="n">
-        <v>0.5108695652173914</v>
+        <v>0.4927536231884058</v>
       </c>
       <c r="F150" t="n">
         <v>828</v>
@@ -4518,7 +4518,7 @@
         <v>0.02660632844269484</v>
       </c>
       <c r="E151" t="n">
-        <v>0.4921592279855247</v>
+        <v>0.474065138721351</v>
       </c>
       <c r="F151" t="n">
         <v>828</v>
@@ -4545,7 +4545,7 @@
         <v>0.02243408692747639</v>
       </c>
       <c r="E152" t="n">
-        <v>0.4432367149758454</v>
+        <v>0.5060386473429952</v>
       </c>
       <c r="F152" t="n">
         <v>828</v>
@@ -4572,7 +4572,7 @@
         <v>0.024002957823777</v>
       </c>
       <c r="E153" t="n">
-        <v>0.5060386473429952</v>
+        <v>0.5048309178743962</v>
       </c>
       <c r="F153" t="n">
         <v>828</v>
@@ -4599,7 +4599,7 @@
         <v>0.02531818086086974</v>
       </c>
       <c r="E154" t="n">
-        <v>0.5048309178743962</v>
+        <v>0.4879227053140097</v>
       </c>
       <c r="F154" t="n">
         <v>828</v>
@@ -4626,7 +4626,7 @@
         <v>0.02808568759160049</v>
       </c>
       <c r="E155" t="n">
-        <v>0.4879227053140097</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="F155" t="n">
         <v>828</v>
@@ -4653,7 +4653,7 @@
         <v>0.02762713476002017</v>
       </c>
       <c r="E156" t="n">
-        <v>0.4716525934861279</v>
+        <v>0.4427020506634499</v>
       </c>
       <c r="F156" t="n">
         <v>828</v>
@@ -4680,7 +4680,7 @@
         <v>0.03444115587778578</v>
       </c>
       <c r="E157" t="n">
-        <v>0.4806763285024155</v>
+        <v>0.4830917874396135</v>
       </c>
       <c r="F157" t="n">
         <v>828</v>
@@ -4707,7 +4707,7 @@
         <v>0.03683930323613468</v>
       </c>
       <c r="E158" t="n">
-        <v>0.4830917874396135</v>
+        <v>0.5</v>
       </c>
       <c r="F158" t="n">
         <v>828</v>
@@ -4734,7 +4734,7 @@
         <v>0.0453873558115613</v>
       </c>
       <c r="E159" t="n">
-        <v>0.5</v>
+        <v>0.4758454106280193</v>
       </c>
       <c r="F159" t="n">
         <v>828</v>
@@ -4761,7 +4761,7 @@
         <v>0.03673353377403933</v>
       </c>
       <c r="E160" t="n">
-        <v>0.4758454106280193</v>
+        <v>0.4613526570048309</v>
       </c>
       <c r="F160" t="n">
         <v>828</v>
@@ -4788,7 +4788,7 @@
         <v>0.03683939767290066</v>
       </c>
       <c r="E161" t="n">
-        <v>0.4607961399276236</v>
+        <v>0.4788902291917974</v>
       </c>
       <c r="F161" t="n">
         <v>828</v>
@@ -4809,16 +4809,16 @@
         <v>0</v>
       </c>
       <c r="C162" t="n">
-        <v>0.004977805534588945</v>
+        <v>0.005139180776358662</v>
       </c>
       <c r="D162" t="n">
-        <v>0.03837711811545823</v>
+        <v>0.03898434517638169</v>
       </c>
       <c r="E162" t="n">
-        <v>0.4951690821256038</v>
+        <v>0.5087281795511222</v>
       </c>
       <c r="F162" t="n">
-        <v>828</v>
+        <v>802</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -4836,16 +4836,16 @@
         <v>1</v>
       </c>
       <c r="C163" t="n">
-        <v>0.002964057329484315</v>
+        <v>0.003060148963607248</v>
       </c>
       <c r="D163" t="n">
-        <v>0.03574275169421126</v>
+        <v>0.03631416020113968</v>
       </c>
       <c r="E163" t="n">
-        <v>0.5048309178743962</v>
+        <v>0.4943960149439601</v>
       </c>
       <c r="F163" t="n">
-        <v>828</v>
+        <v>802</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
@@ -4863,16 +4863,16 @@
         <v>2</v>
       </c>
       <c r="C164" t="n">
-        <v>0.00158385356909557</v>
+        <v>0.001633164078718719</v>
       </c>
       <c r="D164" t="n">
-        <v>0.03408388642603696</v>
+        <v>0.0346098776006185</v>
       </c>
       <c r="E164" t="n">
-        <v>0.4951690821256038</v>
+        <v>0.4707347447073474</v>
       </c>
       <c r="F164" t="n">
-        <v>828</v>
+        <v>803</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -4890,16 +4890,16 @@
         <v>3</v>
       </c>
       <c r="C165" t="n">
-        <v>0.0002049859040557752</v>
+        <v>0.0002113677815170385</v>
       </c>
       <c r="D165" t="n">
-        <v>0.03781118199650683</v>
+        <v>0.03839596839646774</v>
       </c>
       <c r="E165" t="n">
-        <v>0.4685990338164251</v>
+        <v>0.489414694894147</v>
       </c>
       <c r="F165" t="n">
-        <v>828</v>
+        <v>803</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -4917,16 +4917,16 @@
         <v>4</v>
       </c>
       <c r="C166" t="n">
-        <v>5.081709674824385e-05</v>
+        <v>5.239919814140212e-05</v>
       </c>
       <c r="D166" t="n">
-        <v>0.02948043011752616</v>
+        <v>0.02993638573079877</v>
       </c>
       <c r="E166" t="n">
-        <v>0.48854041013269</v>
+        <v>0.49813200498132</v>
       </c>
       <c r="F166" t="n">
-        <v>828</v>
+        <v>803</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -4950,7 +4950,7 @@
         <v>0.02724760785592864</v>
       </c>
       <c r="E167" t="n">
-        <v>0.4468599033816425</v>
+        <v>0.5193236714975845</v>
       </c>
       <c r="F167" t="n">
         <v>828</v>
@@ -4977,7 +4977,7 @@
         <v>0.02503909007730733</v>
       </c>
       <c r="E168" t="n">
-        <v>0.5193236714975845</v>
+        <v>0.4915458937198068</v>
       </c>
       <c r="F168" t="n">
         <v>828</v>
@@ -5004,7 +5004,7 @@
         <v>0.02479460715591672</v>
       </c>
       <c r="E169" t="n">
-        <v>0.4915458937198068</v>
+        <v>0.4855072463768116</v>
       </c>
       <c r="F169" t="n">
         <v>828</v>
@@ -5031,7 +5031,7 @@
         <v>0.02705987436507663</v>
       </c>
       <c r="E170" t="n">
-        <v>0.4855072463768116</v>
+        <v>0.5060386473429952</v>
       </c>
       <c r="F170" t="n">
         <v>828</v>
@@ -5058,7 +5058,7 @@
         <v>0.02407180963407856</v>
       </c>
       <c r="E171" t="n">
-        <v>0.5054282267792521</v>
+        <v>0.4463208685162847</v>
       </c>
       <c r="F171" t="n">
         <v>828</v>
@@ -5085,7 +5085,7 @@
         <v>0.02790253604782945</v>
       </c>
       <c r="E172" t="n">
-        <v>0.4420289855072464</v>
+        <v>0.4782608695652174</v>
       </c>
       <c r="F172" t="n">
         <v>828</v>
@@ -5112,7 +5112,7 @@
         <v>0.03081358261392325</v>
       </c>
       <c r="E173" t="n">
-        <v>0.4782608695652174</v>
+        <v>0.4879227053140097</v>
       </c>
       <c r="F173" t="n">
         <v>828</v>
@@ -5139,7 +5139,7 @@
         <v>0.03332920389191043</v>
       </c>
       <c r="E174" t="n">
-        <v>0.4879227053140097</v>
+        <v>0.4480676328502415</v>
       </c>
       <c r="F174" t="n">
         <v>828</v>
@@ -5166,7 +5166,7 @@
         <v>0.03111962600951647</v>
       </c>
       <c r="E175" t="n">
-        <v>0.4480676328502415</v>
+        <v>0.4661835748792271</v>
       </c>
       <c r="F175" t="n">
         <v>828</v>
@@ -5193,7 +5193,7 @@
         <v>0.02748828774078969</v>
       </c>
       <c r="E176" t="n">
-        <v>0.46562123039807</v>
+        <v>0.4414957780458383</v>
       </c>
       <c r="F176" t="n">
         <v>828</v>
@@ -5220,7 +5220,7 @@
         <v>0.02532719258471252</v>
       </c>
       <c r="E177" t="n">
-        <v>0.4528985507246377</v>
+        <v>0.5253623188405797</v>
       </c>
       <c r="F177" t="n">
         <v>828</v>
@@ -5247,7 +5247,7 @@
         <v>0.02695624141970166</v>
       </c>
       <c r="E178" t="n">
-        <v>0.5253623188405797</v>
+        <v>0.4830917874396135</v>
       </c>
       <c r="F178" t="n">
         <v>828</v>
@@ -5274,7 +5274,7 @@
         <v>0.0293415481563952</v>
       </c>
       <c r="E179" t="n">
-        <v>0.4830917874396135</v>
+        <v>0.5060386473429952</v>
       </c>
       <c r="F179" t="n">
         <v>828</v>
@@ -5301,7 +5301,7 @@
         <v>0.03136032458978902</v>
       </c>
       <c r="E180" t="n">
-        <v>0.5060386473429952</v>
+        <v>0.5241545893719807</v>
       </c>
       <c r="F180" t="n">
         <v>828</v>
@@ -5328,7 +5328,7 @@
         <v>0.02469120602782483</v>
       </c>
       <c r="E181" t="n">
-        <v>0.5235223160434258</v>
+        <v>0.4523522316043426</v>
       </c>
       <c r="F181" t="n">
         <v>828</v>
@@ -5355,7 +5355,7 @@
         <v>0.02760875038911807</v>
       </c>
       <c r="E182" t="n">
-        <v>0.4190821256038647</v>
+        <v>0.5024154589371981</v>
       </c>
       <c r="F182" t="n">
         <v>828</v>
@@ -5382,7 +5382,7 @@
         <v>0.02641331923018986</v>
       </c>
       <c r="E183" t="n">
-        <v>0.5024154589371981</v>
+        <v>0.4806763285024155</v>
       </c>
       <c r="F183" t="n">
         <v>828</v>
@@ -5409,7 +5409,7 @@
         <v>0.02448997667989997</v>
       </c>
       <c r="E184" t="n">
-        <v>0.4806763285024155</v>
+        <v>0.4975845410628019</v>
       </c>
       <c r="F184" t="n">
         <v>828</v>
@@ -5436,7 +5436,7 @@
         <v>0.02258543009747926</v>
       </c>
       <c r="E185" t="n">
-        <v>0.4975845410628019</v>
+        <v>0.5157004830917874</v>
       </c>
       <c r="F185" t="n">
         <v>828</v>
@@ -5463,7 +5463,7 @@
         <v>0.0308799327185528</v>
       </c>
       <c r="E186" t="n">
-        <v>0.5150784077201448</v>
+        <v>0.4185765983112184</v>
       </c>
       <c r="F186" t="n">
         <v>828</v>
@@ -5490,7 +5490,7 @@
         <v>0.02157711285092467</v>
       </c>
       <c r="E187" t="n">
-        <v>0.4323671497584541</v>
+        <v>0.46256038647343</v>
       </c>
       <c r="F187" t="n">
         <v>828</v>
@@ -5517,7 +5517,7 @@
         <v>0.02327572761533957</v>
       </c>
       <c r="E188" t="n">
-        <v>0.46256038647343</v>
+        <v>0.4927536231884058</v>
       </c>
       <c r="F188" t="n">
         <v>828</v>
@@ -5544,7 +5544,7 @@
         <v>0.02664684366645923</v>
       </c>
       <c r="E189" t="n">
-        <v>0.4927536231884058</v>
+        <v>0.5060386473429952</v>
       </c>
       <c r="F189" t="n">
         <v>828</v>
@@ -5571,7 +5571,7 @@
         <v>0.0278365401617714</v>
       </c>
       <c r="E190" t="n">
-        <v>0.5060386473429952</v>
+        <v>0.4903381642512077</v>
       </c>
       <c r="F190" t="n">
         <v>828</v>
@@ -5598,7 +5598,7 @@
         <v>0.02720629652948388</v>
       </c>
       <c r="E191" t="n">
-        <v>0.4897466827503016</v>
+        <v>0.4318455971049457</v>
       </c>
       <c r="F191" t="n">
         <v>828</v>
@@ -5625,7 +5625,7 @@
         <v>0.02566665196971767</v>
       </c>
       <c r="E192" t="n">
-        <v>0.4335748792270531</v>
+        <v>0.4891304347826087</v>
       </c>
       <c r="F192" t="n">
         <v>828</v>
@@ -5652,7 +5652,7 @@
         <v>0.0251636647428378</v>
       </c>
       <c r="E193" t="n">
-        <v>0.4891304347826087</v>
+        <v>0.4951690821256038</v>
       </c>
       <c r="F193" t="n">
         <v>828</v>
@@ -5679,7 +5679,7 @@
         <v>0.02647086301726034</v>
       </c>
       <c r="E194" t="n">
-        <v>0.4951690821256038</v>
+        <v>0.4927536231884058</v>
       </c>
       <c r="F194" t="n">
         <v>828</v>
@@ -5706,7 +5706,7 @@
         <v>0.0298311741505231</v>
       </c>
       <c r="E195" t="n">
-        <v>0.4927536231884058</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="F195" t="n">
         <v>828</v>
@@ -5733,7 +5733,7 @@
         <v>0.02706038171752624</v>
       </c>
       <c r="E196" t="n">
-        <v>0.4716525934861279</v>
+        <v>0.4330518697225573</v>
       </c>
       <c r="F196" t="n">
         <v>828</v>
@@ -5760,7 +5760,7 @@
         <v>0.0310512249173025</v>
       </c>
       <c r="E197" t="n">
-        <v>0.4263285024154589</v>
+        <v>0.4806763285024155</v>
       </c>
       <c r="F197" t="n">
         <v>828</v>
@@ -5787,7 +5787,7 @@
         <v>0.02697403481633929</v>
       </c>
       <c r="E198" t="n">
-        <v>0.4806763285024155</v>
+        <v>0.4601449275362319</v>
       </c>
       <c r="F198" t="n">
         <v>828</v>
@@ -5814,7 +5814,7 @@
         <v>0.02724022966527092</v>
       </c>
       <c r="E199" t="n">
-        <v>0.4601449275362319</v>
+        <v>0.4577294685990338</v>
       </c>
       <c r="F199" t="n">
         <v>828</v>
@@ -5868,7 +5868,7 @@
         <v>0.02721444078231552</v>
       </c>
       <c r="E201" t="n">
-        <v>0.4571773220747889</v>
+        <v>0.4258142340168878</v>
       </c>
       <c r="F201" t="n">
         <v>828</v>

</xml_diff>